<commit_message>
Adding all codes for figure reproduction
</commit_message>
<xml_diff>
--- a/table_subjectDemographic_v1.xlsx
+++ b/table_subjectDemographic_v1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Elements/SCI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ismaila/Documents/C-Codes/SCI_GraphTheory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A55E03E-A118-854A-BD3A-F0F50546918A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07208CB-3DEB-8244-8600-972DEFC29E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{530331F0-3408-3642-8B29-4527C487670B}"/>
+    <workbookView xWindow="36220" yWindow="980" windowWidth="30440" windowHeight="18800" activeTab="1" xr2:uid="{530331F0-3408-3642-8B29-4527C487670B}"/>
   </bookViews>
   <sheets>
     <sheet name="Table" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="294">
   <si>
     <t>Notes</t>
   </si>
@@ -915,6 +915,15 @@
   </si>
   <si>
     <t>SCIM (spinal cord independence measure) total score</t>
+  </si>
+  <si>
+    <t>Cervical</t>
+  </si>
+  <si>
+    <t>Thoracic</t>
+  </si>
+  <si>
+    <t>r01</t>
   </si>
 </sst>
 </file>
@@ -980,7 +989,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1032,6 +1041,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1147,7 +1168,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1269,6 +1290,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2205,7 +2238,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2493,7 +2526,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2913,10 +2946,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F811F8-BB36-7E4B-BDA1-44A0144A99DA}">
-  <dimension ref="A1:AO40"/>
+  <dimension ref="A1:AO46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2924,7 +2957,7 @@
     <col min="1" max="1" width="23.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.5" style="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" style="8" customWidth="1"/>
     <col min="5" max="5" width="8.6640625" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.83203125" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" style="8" bestFit="1" customWidth="1"/>
@@ -3092,7 +3125,7 @@
       <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="49" t="s">
         <v>38</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -3213,7 +3246,7 @@
       <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="49" t="s">
         <v>45</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -3334,7 +3367,7 @@
       <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="49" t="s">
         <v>50</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -3455,7 +3488,7 @@
       <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="49" t="s">
         <v>54</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -3576,7 +3609,7 @@
       <c r="B6" s="1">
         <v>5</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="49" t="s">
         <v>59</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -3699,7 +3732,7 @@
       <c r="B7" s="1">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="49" t="s">
         <v>63</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -3820,7 +3853,7 @@
       <c r="B8" s="1">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="49" t="s">
         <v>67</v>
       </c>
       <c r="D8" s="1" t="s">
@@ -3941,7 +3974,7 @@
       <c r="B9" s="1">
         <v>8</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="49" t="s">
         <v>70</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -4062,7 +4095,7 @@
       <c r="B10" s="1">
         <v>9</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="49" t="s">
         <v>72</v>
       </c>
       <c r="D10" s="1" t="s">
@@ -4185,7 +4218,7 @@
       <c r="B11" s="1">
         <v>10</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="49" t="s">
         <v>75</v>
       </c>
       <c r="D11" s="1" t="s">
@@ -4306,7 +4339,7 @@
       <c r="B12" s="1">
         <v>11</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="49" t="s">
         <v>77</v>
       </c>
       <c r="D12" s="1" t="s">
@@ -4427,7 +4460,7 @@
       <c r="B13" s="1">
         <v>12</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="49" t="s">
         <v>80</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -4548,7 +4581,7 @@
       <c r="B14" s="1">
         <v>13</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="49" t="s">
         <v>82</v>
       </c>
       <c r="D14" s="1" t="s">
@@ -4671,7 +4704,7 @@
       <c r="B15" s="1">
         <v>14</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="49" t="s">
         <v>84</v>
       </c>
       <c r="D15" s="7" t="s">
@@ -4794,7 +4827,7 @@
       <c r="B16" s="1">
         <v>15</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="49" t="s">
         <v>87</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -4915,7 +4948,7 @@
       <c r="B17" s="1">
         <v>16</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="49" t="s">
         <v>98</v>
       </c>
       <c r="D17" s="9" t="s">
@@ -5032,7 +5065,7 @@
       <c r="B18" s="26">
         <v>17</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="50" t="s">
         <v>101</v>
       </c>
       <c r="D18" s="26">
@@ -5153,7 +5186,7 @@
       <c r="B19" s="26">
         <v>18</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="50" t="s">
         <v>103</v>
       </c>
       <c r="D19" s="26">
@@ -5274,7 +5307,7 @@
       <c r="B20" s="26">
         <v>19</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="50" t="s">
         <v>105</v>
       </c>
       <c r="D20" s="26">
@@ -5395,7 +5428,7 @@
       <c r="B21" s="26">
         <v>20</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="50" t="s">
         <v>107</v>
       </c>
       <c r="D21" s="26">
@@ -5516,7 +5549,7 @@
       <c r="B22" s="26">
         <v>21</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="50" t="s">
         <v>108</v>
       </c>
       <c r="D22" s="26">
@@ -5637,7 +5670,7 @@
       <c r="B23" s="26">
         <v>22</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="50" t="s">
         <v>110</v>
       </c>
       <c r="D23" s="26">
@@ -5758,7 +5791,7 @@
       <c r="B24" s="26">
         <v>23</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="50" t="s">
         <v>111</v>
       </c>
       <c r="D24" s="26">
@@ -5881,7 +5914,7 @@
       <c r="B25" s="26">
         <v>24</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="50" t="s">
         <v>113</v>
       </c>
       <c r="D25" s="26">
@@ -6002,7 +6035,7 @@
       <c r="B26" s="26">
         <v>25</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="50" t="s">
         <v>115</v>
       </c>
       <c r="D26" s="26">
@@ -6123,7 +6156,7 @@
       <c r="B27" s="26">
         <v>26</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="50" t="s">
         <v>117</v>
       </c>
       <c r="D27" s="26">
@@ -6246,7 +6279,7 @@
       <c r="B28" s="26">
         <v>27</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="50" t="s">
         <v>120</v>
       </c>
       <c r="D28" s="26">
@@ -6367,7 +6400,7 @@
       <c r="B29" s="26">
         <v>28</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="50" t="s">
         <v>125</v>
       </c>
       <c r="D29" s="26" t="s">
@@ -6490,7 +6523,7 @@
       <c r="B30" s="26">
         <v>29</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="50" t="s">
         <v>129</v>
       </c>
       <c r="D30" s="26" t="s">
@@ -6615,7 +6648,7 @@
       <c r="B31" s="26">
         <v>30</v>
       </c>
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="50" t="s">
         <v>134</v>
       </c>
       <c r="D31" s="26" t="s">
@@ -6740,7 +6773,7 @@
       <c r="B32" s="26">
         <v>31</v>
       </c>
-      <c r="C32" s="26" t="s">
+      <c r="C32" s="50" t="s">
         <v>137</v>
       </c>
       <c r="D32" s="26" t="s">
@@ -6863,7 +6896,7 @@
       <c r="B33" s="26">
         <v>32</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="50" t="s">
         <v>141</v>
       </c>
       <c r="D33" s="26" t="s">
@@ -7081,6 +7114,21 @@
       <c r="P40" s="42">
         <f>SUM(P35:P38)</f>
         <v>32</v>
+      </c>
+    </row>
+    <row r="45" spans="1:41">
+      <c r="C45" s="51"/>
+      <c r="D45" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="46" spans="1:41">
+      <c r="C46" s="52"/>
+      <c r="D46" s="8" t="s">
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -7106,7 +7154,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.83203125" defaultRowHeight="16"/>
@@ -7931,7 +7979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B718CB0-2C43-8943-89C8-AB65DFB16876}">
   <dimension ref="A1:H43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
@@ -8850,7 +8898,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -9169,7 +9217,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
Updated with AllegianceMatrx observation
</commit_message>
<xml_diff>
--- a/table_subjectDemographic_v1.xlsx
+++ b/table_subjectDemographic_v1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ismaila/Documents/C-Codes/SCI_GraphTheory/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07208CB-3DEB-8244-8600-972DEFC29E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5E6AC4-B920-FC41-A98E-9FA1DA86B76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36220" yWindow="980" windowWidth="30440" windowHeight="18800" activeTab="1" xr2:uid="{530331F0-3408-3642-8B29-4527C487670B}"/>
   </bookViews>
@@ -923,7 +923,7 @@
     <t>Thoracic</t>
   </si>
   <si>
-    <t>r01</t>
+    <t>r01/r02</t>
   </si>
 </sst>
 </file>
@@ -989,7 +989,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1053,6 +1053,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1168,7 +1192,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1303,6 +1327,24 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="12" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2946,10 +2988,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4F811F8-BB36-7E4B-BDA1-44A0144A99DA}">
-  <dimension ref="A1:AO46"/>
+  <dimension ref="A1:AO48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -3128,7 +3170,7 @@
       <c r="C2" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="54" t="s">
         <v>39</v>
       </c>
       <c r="E2" s="26">
@@ -3249,7 +3291,7 @@
       <c r="C3" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="54" t="s">
         <v>46</v>
       </c>
       <c r="E3" s="26">
@@ -3370,7 +3412,7 @@
       <c r="C4" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="54" t="s">
         <v>51</v>
       </c>
       <c r="E4" s="26">
@@ -3491,7 +3533,7 @@
       <c r="C5" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="54" t="s">
         <v>55</v>
       </c>
       <c r="E5" s="26">
@@ -3612,7 +3654,7 @@
       <c r="C6" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="54" t="s">
         <v>60</v>
       </c>
       <c r="E6" s="26">
@@ -3735,7 +3777,7 @@
       <c r="C7" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" s="54" t="s">
         <v>64</v>
       </c>
       <c r="E7" s="26">
@@ -3856,7 +3898,7 @@
       <c r="C8" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="54" t="s">
         <v>68</v>
       </c>
       <c r="E8" s="26">
@@ -3977,7 +4019,7 @@
       <c r="C9" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="54" t="s">
         <v>71</v>
       </c>
       <c r="E9" s="26">
@@ -4098,7 +4140,7 @@
       <c r="C10" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" s="54" t="s">
         <v>73</v>
       </c>
       <c r="E10" s="26">
@@ -4221,7 +4263,7 @@
       <c r="C11" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="54" t="s">
         <v>76</v>
       </c>
       <c r="E11" s="26">
@@ -4342,7 +4384,7 @@
       <c r="C12" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="54" t="s">
         <v>78</v>
       </c>
       <c r="E12" s="26">
@@ -4463,7 +4505,7 @@
       <c r="C13" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="54" t="s">
         <v>81</v>
       </c>
       <c r="E13" s="26">
@@ -4584,7 +4626,7 @@
       <c r="C14" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" s="54" t="s">
         <v>83</v>
       </c>
       <c r="E14" s="26">
@@ -4707,7 +4749,7 @@
       <c r="C15" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="53" t="s">
         <v>85</v>
       </c>
       <c r="E15" s="28">
@@ -4830,7 +4872,7 @@
       <c r="C16" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="55" t="s">
         <v>88</v>
       </c>
       <c r="E16" s="26">
@@ -4951,7 +4993,7 @@
       <c r="C17" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="56" t="s">
         <v>99</v>
       </c>
       <c r="E17" s="26">
@@ -5068,7 +5110,7 @@
       <c r="C18" s="50" t="s">
         <v>101</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D18" s="57">
         <v>72236</v>
       </c>
       <c r="E18" s="26">
@@ -5189,7 +5231,7 @@
       <c r="C19" s="50" t="s">
         <v>103</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="57">
         <v>95197</v>
       </c>
       <c r="E19" s="26">
@@ -5310,7 +5352,7 @@
       <c r="C20" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="57">
         <v>60970</v>
       </c>
       <c r="E20" s="26">
@@ -5431,7 +5473,7 @@
       <c r="C21" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="D21" s="26">
+      <c r="D21" s="57">
         <v>2432</v>
       </c>
       <c r="E21" s="26">
@@ -5552,7 +5594,7 @@
       <c r="C22" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="D22" s="26">
+      <c r="D22" s="57">
         <v>56297</v>
       </c>
       <c r="E22" s="26">
@@ -5673,7 +5715,7 @@
       <c r="C23" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="D23" s="26">
+      <c r="D23" s="57">
         <v>49349</v>
       </c>
       <c r="E23" s="26">
@@ -5794,7 +5836,7 @@
       <c r="C24" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D24" s="57">
         <v>13152</v>
       </c>
       <c r="E24" s="26">
@@ -5917,7 +5959,7 @@
       <c r="C25" s="50" t="s">
         <v>113</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="57">
         <v>41311</v>
       </c>
       <c r="E25" s="26">
@@ -6038,7 +6080,7 @@
       <c r="C26" s="50" t="s">
         <v>115</v>
       </c>
-      <c r="D26" s="26">
+      <c r="D26" s="57">
         <v>55140</v>
       </c>
       <c r="E26" s="26">
@@ -6159,7 +6201,7 @@
       <c r="C27" s="50" t="s">
         <v>117</v>
       </c>
-      <c r="D27" s="26">
+      <c r="D27" s="57">
         <v>37442</v>
       </c>
       <c r="E27" s="26">
@@ -6282,7 +6324,7 @@
       <c r="C28" s="50" t="s">
         <v>120</v>
       </c>
-      <c r="D28" s="26">
+      <c r="D28" s="57">
         <v>97517</v>
       </c>
       <c r="E28" s="26">
@@ -6403,7 +6445,7 @@
       <c r="C29" s="50" t="s">
         <v>125</v>
       </c>
-      <c r="D29" s="26" t="s">
+      <c r="D29" s="57" t="s">
         <v>126</v>
       </c>
       <c r="E29" s="27">
@@ -6526,7 +6568,7 @@
       <c r="C30" s="50" t="s">
         <v>129</v>
       </c>
-      <c r="D30" s="26" t="s">
+      <c r="D30" s="57" t="s">
         <v>130</v>
       </c>
       <c r="E30" s="26">
@@ -6651,7 +6693,7 @@
       <c r="C31" s="50" t="s">
         <v>134</v>
       </c>
-      <c r="D31" s="26" t="s">
+      <c r="D31" s="58" t="s">
         <v>135</v>
       </c>
       <c r="E31" s="27">
@@ -6776,7 +6818,7 @@
       <c r="C32" s="50" t="s">
         <v>137</v>
       </c>
-      <c r="D32" s="26" t="s">
+      <c r="D32" s="58" t="s">
         <v>138</v>
       </c>
       <c r="E32" s="27">
@@ -6899,7 +6941,7 @@
       <c r="C33" s="50" t="s">
         <v>141</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="D33" s="57" t="s">
         <v>142</v>
       </c>
       <c r="E33" s="26">
@@ -7129,6 +7171,12 @@
       <c r="C46" s="52"/>
       <c r="D46" s="8" t="s">
         <v>292</v>
+      </c>
+    </row>
+    <row r="48" spans="1:41">
+      <c r="C48" s="52"/>
+      <c r="D48" s="8">
+        <v>61375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>